<commit_message>
dramatic change to remove unnecessary folders
</commit_message>
<xml_diff>
--- a/markdown_generator/publications.xlsx
+++ b/markdown_generator/publications.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huiguan/Documents/website/guanh01.github.io/markdown_generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F07557-0C95-A74F-B990-F052F078483D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BAD967-36E6-F14E-999A-08CF2F171F8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35840" yWindow="4400" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="publications" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="77">
   <si>
     <t>pub_date</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Hui Guan, Wen Tang, Hamid Krim, James Keiser, Andrew Rindos, and Radmila Sazdanovic</t>
   </si>
   <si>
-    <t>A topological collapse for document summarization</t>
-  </si>
-  <si>
     <t>spawc</t>
   </si>
   <si>
@@ -82,9 +79,6 @@
     <t>Hui Guan, Xipeng Shen, and Hamid Krim</t>
   </si>
   <si>
-    <t>Egeria: a framework for automatic synthesis of HPC advising tools through multi-layered natural language processing</t>
-  </si>
-  <si>
     <t>sc</t>
   </si>
   <si>
@@ -121,9 +115,6 @@
     <t>Randall Pittman, Hui Guan, Xipeng Shen, Seung-Hwan Lim, and Robert M. Patton</t>
   </si>
   <si>
-    <t>Exploring flexible communications for streamlining DNN ensemble training pipelines</t>
-  </si>
-  <si>
     <t>http://guanh01.github.io/files/2018sc.pdf</t>
   </si>
   <si>
@@ -139,9 +130,6 @@
     <t>Hui Guan, Xipeng Shen, and Seung-Hwan Lim</t>
   </si>
   <si>
-    <t>Wootz: a compiler-based framework for fast CNN pruning via composability</t>
-  </si>
-  <si>
     <t>http://guanh01.github.io/files/2019pldi.pdf</t>
   </si>
   <si>
@@ -223,19 +211,46 @@
     <t>The ACM Joint European Software Engineering Conference and Symposium on the Foundations of Software Engineering (&lt;b&gt;ESEC/FSE&lt;/b&gt;), Sacramento, California, United States, November 2020. (acceptance rate: 101/360=28%) </t>
   </si>
   <si>
-    <t>An automatic synthesizer of advising tools for high performance computing</t>
-  </si>
-  <si>
     <t>IEEE Transactions on Parallel and Distributed Systems (&lt;b&gt;TPDS&lt;/b&gt;)</t>
   </si>
   <si>
     <t>tpds</t>
   </si>
   <si>
-    <t>https://ieeexplore.ieee.org/abstract/document/9173796</t>
-  </si>
-  <si>
-    <t>https://2020.esec-fse.org/details/fse-2020-papers/7/HISyn-Human-Learning-Inspired-Natural-Language-Programming</t>
+    <t>A Topological Collapse for Document Summarization</t>
+  </si>
+  <si>
+    <t>Egeria: a Framework for Automatic Synthesis of HPC Advising Tools through Multi-Layered Natural Language Processing</t>
+  </si>
+  <si>
+    <t>Exploring Flexible Communications for Streamlining DNN Ensemble Training Pipelines</t>
+  </si>
+  <si>
+    <t>Wootz: a Compiler-Based Framework for Fast CNN Pruning via Composability</t>
+  </si>
+  <si>
+    <t>An Automatic Synthesizer of Advising Tools for High Performance Computing</t>
+  </si>
+  <si>
+    <t>http://guanh01.github.io/files/2020tpds.pdf</t>
+  </si>
+  <si>
+    <t>http://guanh01.github.io/files/2020hisyn.pdf</t>
+  </si>
+  <si>
+    <t>Zifan Nan, Hui Guan, Xipeng Shen, and Chunhua Liao</t>
+  </si>
+  <si>
+    <t>Deep NLP-Based Co-Evolvement for Synthesizing Code Analysis from Natural Language</t>
+  </si>
+  <si>
+    <t>The ACM SIGPLAN 2021 International Conference on Compiler Construction (&lt;b&gt;CC 2021&lt;/b&gt;)</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t>http://guanh01.github.io/files/2021cc.pdf</t>
   </si>
 </sst>
 </file>
@@ -245,7 +260,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -384,6 +399,14 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val=".AppleSystemUIFont"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -683,7 +706,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -726,13 +749,17 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -766,6 +793,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1086,10 +1114,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1097,7 +1125,7 @@
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="63.5" customWidth="1"/>
     <col min="3" max="3" width="56.83203125" customWidth="1"/>
-    <col min="4" max="4" width="56" customWidth="1"/>
+    <col min="4" max="4" width="90.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1121,286 +1149,311 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>42522</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>42705</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>42736</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>43053</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>43132</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>43344</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
+        <v>43405</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1">
+        <v>43617</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1">
+        <v>43627</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" t="s">
         <v>59</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="2">
-        <v>42705</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="2">
-        <v>42736</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="E10" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="2">
-        <v>43053</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="2">
-        <v>43132</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="2">
-        <v>43344</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="F10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1">
+        <v>43808</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
         <v>60</v>
       </c>
-      <c r="E7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="2">
-        <v>43405</v>
-      </c>
-      <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1">
+        <v>43808</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1">
+        <v>43894</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
         <v>61</v>
       </c>
-      <c r="E8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="2">
-        <v>43617</v>
-      </c>
-      <c r="B9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1">
+        <v>44136</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" t="s">
         <v>62</v>
       </c>
-      <c r="E9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="2">
-        <v>43627</v>
-      </c>
-      <c r="B10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="2">
-        <v>43808</v>
-      </c>
-      <c r="B11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="2">
-        <v>43808</v>
-      </c>
-      <c r="B12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="2">
-        <v>43894</v>
-      </c>
-      <c r="B13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>52</v>
       </c>
-      <c r="F13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="2">
-        <v>44136</v>
-      </c>
-      <c r="B14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" t="s">
-        <v>66</v>
-      </c>
-      <c r="E14" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="F14" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1">
-        <v>44137</v>
+        <v>44136</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E15" t="s">
-        <v>69</v>
-      </c>
-      <c r="F15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>70</v>
       </c>
     </row>
+    <row r="16" spans="1:6" ht="34">
+      <c r="A16" s="1">
+        <v>44197</v>
+      </c>
+      <c r="B16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F15" r:id="rId1" xr:uid="{D7B64B95-9D14-1F4C-8997-3F0170E8D006}"/>
+    <hyperlink ref="F14" r:id="rId2" xr:uid="{7C0B6682-E7FC-A240-A886-6C99B6750C8A}"/>
+    <hyperlink ref="F16" r:id="rId3" xr:uid="{4054A136-F4CC-D544-8E1E-C1E6E1280599}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>